<commit_message>
add charactor limit about bio input
</commit_message>
<xml_diff>
--- a/dist/goods_modelo.xlsx
+++ b/dist/goods_modelo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25480" windowHeight="14040"/>
+    <workbookView windowWidth="17700" windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>名称</t>
   </si>
@@ -80,21 +80,43 @@
     <t>测试</t>
   </si>
   <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
     <t>测试2</t>
   </si>
   <si>
+    <t>Caja</t>
+  </si>
+  <si>
     <t>测试3</t>
+  </si>
+  <si>
+    <t>Paquete</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>Palet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -249,12 +271,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -575,7 +603,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -599,16 +627,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -617,90 +645,109 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1228,96 +1275,279 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="9" max="9" width="13.2980769230769" customWidth="1"/>
-    <col min="10" max="10" width="16.3365384615385" customWidth="1"/>
-    <col min="11" max="11" width="15.375" customWidth="1"/>
-    <col min="12" max="12" width="13.2980769230769" customWidth="1"/>
-    <col min="14" max="14" width="13.4519230769231" customWidth="1"/>
+    <col min="1" max="4" width="9.23076923076923" style="1"/>
+    <col min="5" max="8" width="9.23076923076923" style="2"/>
+    <col min="9" max="9" width="13.2980769230769" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.3365384615385" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.2980769230769" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.23076923076923" style="1"/>
+    <col min="14" max="14" width="13.4519230769231" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2.01</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>11111</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2.01</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="L3" s="3">
+        <v>4.01</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1">
+        <v>22222</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
         <v>3</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.01</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4.01</v>
+      </c>
+      <c r="L4" s="3">
+        <v>5.01</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1">
+        <v>100</v>
+      </c>
+      <c r="P4" s="1">
+        <v>33333</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2">
+        <v>55</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.01</v>
+      </c>
+      <c r="K5" s="3">
+        <v>5.01</v>
+      </c>
+      <c r="L5" s="3">
+        <v>6.01</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P5" s="1">
+        <v>44444</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="15:15">
+      <c r="O15" s="5"/>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Solo se puede elejir uno" prompt="Unidad, Caja, Paquete, Palet" sqref="M1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Solo se puede elejir uno" prompt="Unidad, Caja, Paquete, Palet" sqref="M2:M1048576">
+      <formula1>$S$2:$S$5</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="错误" error="必须大于或者等于0" sqref="N2:N1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="错误" error="必须大于或者等于0" sqref="P2:P1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>